<commit_message>
Se mejoro los logs para mastertable, ademas los logs se descargan independiente mente que sea o no exitoso la carga de las mastertables
</commit_message>
<xml_diff>
--- a/apidev/MasterTablesGenerada_v1.xlsx
+++ b/apidev/MasterTablesGenerada_v1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="1352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="1341">
   <si>
     <t>WAV</t>
   </si>
@@ -3972,18 +3972,6 @@
     <t>CAJA PLASTICA SEGUN FOTO CAMILO.JPG</t>
   </si>
   <si>
-    <t>MICROFONO INTEGRADO</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH EXTERNO</t>
-  </si>
-  <si>
-    <t>SMX-II</t>
-  </si>
-  <si>
-    <t>SENNHEISER DIRECCIONAL</t>
-  </si>
-  <si>
     <t>MICRO SD</t>
   </si>
   <si>
@@ -4048,27 +4036,6 @@
   </si>
   <si>
     <t>LLUVIOSA</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH GANANCIA BAJA</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH GANANCIA BAJA-MEDIA</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH GANANCIA MEDIA</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH GANANCIA MEDIA-ALTA</t>
-  </si>
-  <si>
-    <t>AUDIOMOTH GANANCIA ALTA</t>
-  </si>
-  <si>
-    <t>16DB</t>
-  </si>
-  <si>
-    <t>SM4 SIN GANANCIA</t>
   </si>
   <si>
     <t>GHA</t>
@@ -4454,17 +4421,17 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
     </row>
   </sheetData>
@@ -4487,27 +4454,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
     </row>
   </sheetData>
@@ -4530,7 +4497,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4515,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
     </row>
   </sheetData>
@@ -4576,32 +4543,32 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -4611,7 +4578,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
     </row>
   </sheetData>
@@ -4634,22 +4601,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
     </row>
   </sheetData>
@@ -4659,53 +4626,12 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4737,32 +4663,32 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1346</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1348</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1349</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1350</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>1351</v>
+        <v>1340</v>
       </c>
     </row>
   </sheetData>
@@ -11538,38 +11464,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se descargan los logs cuando se crga el udas salga o no error
</commit_message>
<xml_diff>
--- a/apidev/MasterTablesGenerada_v1.xlsx
+++ b/apidev/MasterTablesGenerada_v1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="1341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="1356">
   <si>
     <t>WAV</t>
   </si>
@@ -3972,6 +3972,18 @@
     <t>CAJA PLASTICA SEGUN FOTO CAMILO.JPG</t>
   </si>
   <si>
+    <t>MICROFONO INTEGRADO</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH EXTERNO</t>
+  </si>
+  <si>
+    <t>SMX-II</t>
+  </si>
+  <si>
+    <t>SENNHEISER DIRECCIONAL</t>
+  </si>
+  <si>
     <t>MICRO SD</t>
   </si>
   <si>
@@ -4038,6 +4050,36 @@
     <t>LLUVIOSA</t>
   </si>
   <si>
+    <t>AUDIOMOTH GANANCIA BAJA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH GANANCIA BAJA-MEDIA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH GANANCIA MEDIA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH GANANCIA MEDIA-ALTA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH GANANCIA ALTA</t>
+  </si>
+  <si>
+    <t>16DB</t>
+  </si>
+  <si>
+    <t>SM4 SIN GANANCIA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH SIN GANANCIA</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH SIN GANANCIA 2</t>
+  </si>
+  <si>
+    <t>AUDIOMOTH SIN GANANCIA 3</t>
+  </si>
+  <si>
     <t>GHA</t>
   </si>
   <si>
@@ -4054,6 +4096,9 @@
   </si>
   <si>
     <t>GHA-ISAGEN-COLCIENCIAS</t>
+  </si>
+  <si>
+    <t>ECOPETROL</t>
   </si>
 </sst>
 </file>
@@ -4421,17 +4466,17 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1313</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1314</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1315</v>
+        <v>1319</v>
       </c>
     </row>
   </sheetData>
@@ -4454,27 +4499,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1316</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1317</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1318</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1319</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1320</v>
+        <v>1324</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4542,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
     </row>
   </sheetData>
@@ -4515,12 +4560,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1322</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1323</v>
+        <v>1327</v>
       </c>
     </row>
   </sheetData>
@@ -4543,32 +4588,32 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1324</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1325</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1326</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1327</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>1329</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -4578,7 +4623,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>1330</v>
+        <v>1334</v>
       </c>
     </row>
   </sheetData>
@@ -4601,22 +4646,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1331</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1332</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1333</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1334</v>
+        <v>1338</v>
       </c>
     </row>
   </sheetData>
@@ -4626,12 +4671,68 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4650,7 +4751,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4663,32 +4764,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1335</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1336</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1337</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1338</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1339</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>1340</v>
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>1355</v>
       </c>
     </row>
   </sheetData>
@@ -11338,7 +11444,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11401,11 +11507,6 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
         <v>1306</v>
       </c>
     </row>
@@ -11464,12 +11565,38 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>